<commit_message>
remade import program using custom command
</commit_message>
<xml_diff>
--- a/settlements.xlsx
+++ b/settlements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\GEO_dm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132C61DC-B6D6-4104-ABA4-0542C11F026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BABEFFD-ACD7-4EC5-9560-2E66A69576B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="384">
   <si>
     <t>SETTLEP</t>
   </si>
@@ -1176,19 +1176,22 @@
     <t>Shelter</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>name</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>type</t>
   </si>
   <si>
-    <t>ParishCode</t>
+    <t>parish</t>
   </si>
   <si>
-    <t>Longitude</t>
+    <t>code</t>
   </si>
   <si>
-    <t>Latitude</t>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,16 +1700,16 @@
         <v>379</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>380</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>

</xml_diff>